<commit_message>
Türklerde Eksik Kalan Haziran Hakedişleri Eklendi
</commit_message>
<xml_diff>
--- a/Ofis Dosyalari/HAKEDISLER/2025/AĞUSTOS 2025/2025 AĞUSTOS AYI - TÜRKLER.xlsx
+++ b/Ofis Dosyalari/HAKEDISLER/2025/AĞUSTOS 2025/2025 AĞUSTOS AYI - TÜRKLER.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samil\OneDrive\Desktop\OfisDosyalariYedegi\Ofis Dosyalari\HAKEDISLER\2025\AĞUSTOS 2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4C53A7-F4CF-4A0C-98AD-786DA6C442C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD70D8D-E214-4A5B-A069-E11B61A40B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -462,9 +462,11 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
         <color auto="1"/>
@@ -475,7 +477,9 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color auto="1"/>
       </top>
@@ -488,12 +492,14 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -502,7 +508,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -573,15 +579,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -591,10 +588,28 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -879,7 +894,7 @@
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4"/>
@@ -900,21 +915,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
     </row>
     <row r="2" spans="1:14" ht="43.8" thickBot="1">
       <c r="A2" s="1" t="s">
@@ -969,22 +984,24 @@
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
+      <c r="F3" s="7">
+        <v>1883</v>
+      </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7">
         <v>2500</v>
       </c>
       <c r="I3" s="8">
-        <f>H3*M3</f>
-        <v>212500</v>
+        <f>(F3+H3)*M3</f>
+        <v>372555</v>
       </c>
       <c r="J3" s="8"/>
-      <c r="K3" s="8">
+      <c r="K3" s="34">
         <f t="shared" ref="K3:K14" si="0">I3-J3</f>
-        <v>212500</v>
-      </c>
-      <c r="L3" s="26"/>
-      <c r="M3" s="29">
+        <v>372555</v>
+      </c>
+      <c r="L3" s="31"/>
+      <c r="M3" s="26">
         <v>85</v>
       </c>
     </row>
@@ -1000,22 +1017,24 @@
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
+      <c r="F4" s="13">
+        <v>1142</v>
+      </c>
       <c r="G4" s="13"/>
       <c r="H4" s="13">
         <v>2500</v>
       </c>
       <c r="I4" s="14">
-        <f>H4*M4</f>
-        <v>212500</v>
+        <f>(F4+H4)*M4</f>
+        <v>309570</v>
       </c>
       <c r="J4" s="14"/>
-      <c r="K4" s="14">
+      <c r="K4" s="35">
         <f t="shared" si="0"/>
-        <v>212500</v>
-      </c>
-      <c r="L4" s="27"/>
-      <c r="M4" s="30">
+        <v>309570</v>
+      </c>
+      <c r="L4" s="32"/>
+      <c r="M4" s="27">
         <v>85</v>
       </c>
     </row>
@@ -1044,16 +1063,16 @@
         <v>3622</v>
       </c>
       <c r="I5" s="14">
-        <f>H5*M5</f>
+        <f t="shared" ref="I3:I8" si="1">H5*M5</f>
         <v>307870</v>
       </c>
       <c r="J5" s="14"/>
-      <c r="K5" s="14">
+      <c r="K5" s="35">
         <f t="shared" si="0"/>
         <v>307870</v>
       </c>
-      <c r="L5" s="27"/>
-      <c r="M5" s="30">
+      <c r="L5" s="32"/>
+      <c r="M5" s="27">
         <v>85</v>
       </c>
     </row>
@@ -1078,20 +1097,20 @@
       </c>
       <c r="G6" s="13"/>
       <c r="H6" s="13">
-        <f t="shared" ref="H6:H13" si="1">(D6*E6)+F6+G6</f>
+        <f t="shared" ref="H6:H13" si="2">(D6*E6)+F6+G6</f>
         <v>3552</v>
       </c>
       <c r="I6" s="14">
-        <f>H6*M6</f>
+        <f t="shared" si="1"/>
         <v>301920</v>
       </c>
       <c r="J6" s="14"/>
-      <c r="K6" s="14">
+      <c r="K6" s="35">
         <f t="shared" si="0"/>
         <v>301920</v>
       </c>
-      <c r="L6" s="27"/>
-      <c r="M6" s="30">
+      <c r="L6" s="32"/>
+      <c r="M6" s="27">
         <v>85</v>
       </c>
     </row>
@@ -1114,20 +1133,20 @@
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
       <c r="H7" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I7" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I7" s="14">
-        <f>H7*M7</f>
-        <v>0</v>
-      </c>
       <c r="J7" s="14"/>
-      <c r="K7" s="14">
+      <c r="K7" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L7" s="27"/>
-      <c r="M7" s="30">
+      <c r="L7" s="32"/>
+      <c r="M7" s="27">
         <v>85</v>
       </c>
     </row>
@@ -1154,20 +1173,20 @@
         <v>2660</v>
       </c>
       <c r="H8" s="13">
+        <f t="shared" si="2"/>
+        <v>6359</v>
+      </c>
+      <c r="I8" s="14">
         <f t="shared" si="1"/>
-        <v>6359</v>
-      </c>
-      <c r="I8" s="14">
-        <f>H8*M8</f>
         <v>540515</v>
       </c>
       <c r="J8" s="14"/>
-      <c r="K8" s="14">
+      <c r="K8" s="35">
         <f t="shared" si="0"/>
         <v>540515</v>
       </c>
-      <c r="L8" s="27"/>
-      <c r="M8" s="30">
+      <c r="L8" s="32"/>
+      <c r="M8" s="27">
         <v>85</v>
       </c>
     </row>
@@ -1192,20 +1211,20 @@
       </c>
       <c r="G9" s="13"/>
       <c r="H9" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3377</v>
       </c>
       <c r="I9" s="14">
-        <f t="shared" ref="I9:I14" si="2">H9*M9</f>
+        <f t="shared" ref="I9:I14" si="3">H9*M9</f>
         <v>287045</v>
       </c>
       <c r="J9" s="14"/>
-      <c r="K9" s="14">
+      <c r="K9" s="35">
         <f t="shared" si="0"/>
         <v>287045</v>
       </c>
-      <c r="L9" s="27"/>
-      <c r="M9" s="30">
+      <c r="L9" s="32"/>
+      <c r="M9" s="27">
         <v>85</v>
       </c>
     </row>
@@ -1227,16 +1246,16 @@
         <v>2000</v>
       </c>
       <c r="I10" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>170000</v>
       </c>
       <c r="J10" s="14"/>
-      <c r="K10" s="14">
+      <c r="K10" s="35">
         <f t="shared" si="0"/>
         <v>170000</v>
       </c>
-      <c r="L10" s="27"/>
-      <c r="M10" s="30">
+      <c r="L10" s="32"/>
+      <c r="M10" s="27">
         <v>85</v>
       </c>
     </row>
@@ -1261,23 +1280,23 @@
       </c>
       <c r="G11" s="13"/>
       <c r="H11" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3803</v>
       </c>
       <c r="I11" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>323255</v>
       </c>
       <c r="J11" s="14"/>
-      <c r="K11" s="14">
+      <c r="K11" s="35">
         <f t="shared" si="0"/>
         <v>323255</v>
       </c>
-      <c r="L11" s="27"/>
-      <c r="M11" s="30">
+      <c r="L11" s="32"/>
+      <c r="M11" s="27">
         <v>85</v>
       </c>
-      <c r="N11" s="33" t="s">
+      <c r="N11" s="29" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1297,23 +1316,25 @@
       <c r="E12" s="13">
         <v>7</v>
       </c>
-      <c r="F12" s="13"/>
+      <c r="F12" s="13">
+        <v>597</v>
+      </c>
       <c r="G12" s="13"/>
       <c r="H12" s="13">
-        <f t="shared" si="1"/>
-        <v>973</v>
+        <f t="shared" si="2"/>
+        <v>1570</v>
       </c>
       <c r="I12" s="14">
-        <f t="shared" si="2"/>
-        <v>82705</v>
+        <f t="shared" si="3"/>
+        <v>133450</v>
       </c>
       <c r="J12" s="14"/>
-      <c r="K12" s="14">
+      <c r="K12" s="35">
         <f t="shared" si="0"/>
-        <v>82705</v>
-      </c>
-      <c r="L12" s="27"/>
-      <c r="M12" s="30">
+        <v>133450</v>
+      </c>
+      <c r="L12" s="32"/>
+      <c r="M12" s="27">
         <v>85</v>
       </c>
     </row>
@@ -1338,20 +1359,20 @@
       </c>
       <c r="G13" s="13"/>
       <c r="H13" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2273</v>
       </c>
       <c r="I13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>193205</v>
       </c>
       <c r="J13" s="14"/>
-      <c r="K13" s="14">
+      <c r="K13" s="35">
         <f t="shared" si="0"/>
         <v>193205</v>
       </c>
-      <c r="L13" s="27"/>
-      <c r="M13" s="30">
+      <c r="L13" s="32"/>
+      <c r="M13" s="27">
         <v>85</v>
       </c>
     </row>
@@ -1373,18 +1394,18 @@
         <v>1000</v>
       </c>
       <c r="I14" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>85000</v>
       </c>
       <c r="J14" s="22">
         <v>20000</v>
       </c>
-      <c r="K14" s="22">
+      <c r="K14" s="36">
         <f t="shared" si="0"/>
         <v>65000</v>
       </c>
-      <c r="L14" s="28"/>
-      <c r="M14" s="31">
+      <c r="L14" s="33"/>
+      <c r="M14" s="28">
         <v>85</v>
       </c>
     </row>
@@ -1392,13 +1413,13 @@
     <row r="16" spans="1:14" ht="15" thickBot="1">
       <c r="H16" s="23">
         <f>SUM(H3:H15)</f>
-        <v>31959</v>
+        <v>32556</v>
       </c>
       <c r="I16" s="24"/>
       <c r="J16" s="24"/>
       <c r="K16" s="25">
         <f>SUM(K3:K15)</f>
-        <v>2696515</v>
+        <v>3004385</v>
       </c>
     </row>
   </sheetData>

</xml_diff>